<commit_message>
Experimentation with merging dataframes
</commit_message>
<xml_diff>
--- a/H_SK_PRD.xlsx
+++ b/H_SK_PRD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.17.152.102\ftp\Adam_ftp\H_SK post_changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.17.152.102\ftp\Adam_ftp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -570,7 +570,7 @@
     <t>Remote Information</t>
   </si>
   <si>
-    <t>Analog &amp; Tank(T) Points List generated at 2023/01/30 09:50</t>
+    <t>Analog &amp; Tank(T) Points List generated at 2023/01/30 09:35</t>
   </si>
   <si>
     <t>Pembina Pipeline Corp.</t>
@@ -594,7 +594,7 @@
     <t>Rate Name</t>
   </si>
   <si>
-    <t>Rate Points List generated at 2023/01/30 09:50</t>
+    <t>Rate Points List generated at 2023/01/30 09:35</t>
   </si>
   <si>
     <t>OPP/F</t>
@@ -2184,7 +2184,7 @@
     <t>Status Name</t>
   </si>
   <si>
-    <t>Status/Digital Points List generated at 2023/01/30 09:50</t>
+    <t>Status/Digital Points List generated at 2023/01/30 09:35</t>
   </si>
 </sst>
 </file>

</xml_diff>